<commit_message>
Deploying to gh-pages from @ NIH-NCPI/ncpi-fhir-ig@8c2cc6a1c26501b94f0d660124b8b21af2005902 🚀
</commit_message>
<xml_diff>
--- a/ValueSet-condition-inheritance-vs.xlsx
+++ b/ValueSet-condition-inheritance-vs.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Include from Condition Inherita" r:id="rId4" sheetId="2"/>
+    <sheet name="Include from Condition Inheri" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-09-14T17:59:16+00:00</t>
+    <t>2021-12-13T19:23:29+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>